<commit_message>
Correzione User Story 2
</commit_message>
<xml_diff>
--- a/PreGame-FirstSprintPlanning.xlsx
+++ b/PreGame-FirstSprintPlanning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annamaria\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9839d344ee2d2222/Documenti/GitHub/ProgettoSEGruppo16-IZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9417685F-5B7B-4348-81B6-A50B7BDCD80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9417685F-5B7B-4348-81B6-A50B7BDCD80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4B5177E-8AC3-4F40-8FF5-F1A1F511C7BE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="612" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="81">
   <si>
     <t>#ID</t>
   </si>
@@ -80,9 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">Come utente, voglio che l'applicazione controlli periodicamente le regole in modo da valutare automaticamente se i trigger sono attivati. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Dopo che è stata aggiunta una regola, viene verificata automaticamente la condizione del trigger ogni 5 secondi </t>
   </si>
   <si>
     <t>Come utente, voglio specificare come trigger un particolare orario del giorno in modo che l'azione venga eseguita al tempo specificato.</t>
@@ -386,6 +381,12 @@
       </rPr>
       <t xml:space="preserve"> 48</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Come utente, voglio che l'applicazione controlli periodicamente le regole ogni 5 secondi in modo da valutare automaticamente se i trigger sono attivati. </t>
+  </si>
+  <si>
+    <t>- Dopo che è stata aggiunta una regola, la verifica delle regole avviene in maniera automatica, senza interazione da parte dell'utente.</t>
   </si>
 </sst>
 </file>
@@ -912,9 +913,9 @@
   </sheetPr>
   <dimension ref="A1:AC1013"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1029,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="C3" s="24">
         <v>1</v>
@@ -1044,7 +1045,7 @@
       </c>
       <c r="G3" s="25"/>
       <c r="H3" s="45" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1073,7 +1074,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="24">
         <v>2</v>
@@ -1089,7 +1090,7 @@
       </c>
       <c r="G4" s="25"/>
       <c r="H4" s="45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1118,7 +1119,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="24">
         <v>2</v>
@@ -1134,7 +1135,7 @@
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1163,7 +1164,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="24">
         <v>2</v>
@@ -1179,7 +1180,7 @@
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" s="1"/>
       <c r="K6" s="1"/>
@@ -1238,7 +1239,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="24">
         <v>3</v>
@@ -1254,7 +1255,7 @@
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1283,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="24">
         <v>4</v>
@@ -1299,7 +1300,7 @@
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1328,7 +1329,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="24">
         <v>3</v>
@@ -1344,7 +1345,7 @@
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1373,7 +1374,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="24">
         <v>5</v>
@@ -1389,7 +1390,7 @@
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1449,7 +1450,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="15">
         <v>6</v>
@@ -1459,7 +1460,7 @@
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="31"/>
       <c r="H13" s="13"/>
@@ -1490,7 +1491,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="15">
         <v>6</v>
@@ -1500,7 +1501,7 @@
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="13"/>
@@ -1531,7 +1532,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="15">
         <v>6</v>
@@ -1541,7 +1542,7 @@
       </c>
       <c r="E15" s="31"/>
       <c r="F15" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="31"/>
       <c r="H15" s="31"/>
@@ -1572,7 +1573,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="15">
         <v>6</v>
@@ -1582,7 +1583,7 @@
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
@@ -1613,7 +1614,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="15">
         <v>7</v>
@@ -1623,7 +1624,7 @@
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
@@ -1654,7 +1655,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="15">
         <v>6</v>
@@ -1664,7 +1665,7 @@
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
@@ -1695,7 +1696,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="15">
         <v>6</v>
@@ -1705,7 +1706,7 @@
       </c>
       <c r="E19" s="31"/>
       <c r="F19" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" s="31"/>
       <c r="H19" s="31"/>
@@ -1736,7 +1737,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="15">
         <v>6</v>
@@ -1746,7 +1747,7 @@
       </c>
       <c r="E20" s="31"/>
       <c r="F20" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" s="31"/>
       <c r="H20" s="31"/>
@@ -1777,7 +1778,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="15">
         <v>6</v>
@@ -1787,7 +1788,7 @@
       </c>
       <c r="E21" s="31"/>
       <c r="F21" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
@@ -1818,7 +1819,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="15">
         <v>6</v>
@@ -1828,7 +1829,7 @@
       </c>
       <c r="E22" s="31"/>
       <c r="F22" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="31"/>
       <c r="H22" s="31"/>
@@ -1859,7 +1860,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="15">
         <v>7</v>
@@ -1869,7 +1870,7 @@
       </c>
       <c r="E23" s="31"/>
       <c r="F23" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -1930,7 +1931,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="15">
         <v>8</v>
@@ -1940,7 +1941,7 @@
       </c>
       <c r="E25" s="31"/>
       <c r="F25" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -1971,7 +1972,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="15">
         <v>8</v>
@@ -1981,7 +1982,7 @@
       </c>
       <c r="E26" s="35"/>
       <c r="F26" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G26" s="36"/>
       <c r="H26" s="36"/>
@@ -2043,7 +2044,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="12">
         <v>9</v>
@@ -2053,7 +2054,7 @@
       </c>
       <c r="E28" s="35"/>
       <c r="F28" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G28" s="36"/>
       <c r="H28" s="36"/>
@@ -2084,7 +2085,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="12">
         <v>9</v>
@@ -2094,7 +2095,7 @@
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="36"/>
@@ -2125,7 +2126,7 @@
         <v>25</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="12">
         <v>10</v>
@@ -2135,7 +2136,7 @@
       </c>
       <c r="E30" s="35"/>
       <c r="F30" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30" s="36"/>
       <c r="H30" s="36"/>
@@ -2166,7 +2167,7 @@
         <v>26</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="12">
         <v>10</v>
@@ -2176,7 +2177,7 @@
       </c>
       <c r="E31" s="35"/>
       <c r="F31" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G31" s="36"/>
       <c r="H31" s="36"/>
@@ -2207,7 +2208,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="12">
         <v>10</v>
@@ -2217,7 +2218,7 @@
       </c>
       <c r="E32" s="35"/>
       <c r="F32" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G32" s="36"/>
       <c r="H32" s="36"/>
@@ -2248,7 +2249,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="12">
         <v>10</v>
@@ -2258,7 +2259,7 @@
       </c>
       <c r="E33" s="35"/>
       <c r="F33" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G33" s="36"/>
       <c r="H33" s="36"/>
@@ -2289,7 +2290,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="12">
         <v>10</v>
@@ -2299,7 +2300,7 @@
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G34" s="36"/>
       <c r="H34" s="36"/>
@@ -2330,7 +2331,7 @@
         <v>30</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="12">
         <v>11</v>
@@ -2340,7 +2341,7 @@
       </c>
       <c r="E35" s="35"/>
       <c r="F35" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G35" s="36"/>
       <c r="H35" s="36"/>
@@ -32705,7 +32706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702733D5-5995-4FC8-88D3-37A467A289D6}">
   <dimension ref="A1:H1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -32758,14 +32759,14 @@
       </c>
       <c r="F2" s="27"/>
       <c r="H2" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="15"/>
       <c r="C3" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="15"/>
@@ -32775,7 +32776,7 @@
       <c r="A4" s="15"/>
       <c r="B4" s="15"/>
       <c r="C4" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="15"/>
@@ -32785,7 +32786,7 @@
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="15"/>
@@ -32795,7 +32796,7 @@
       <c r="A6" s="15"/>
       <c r="B6" s="15"/>
       <c r="C6" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="15"/>
@@ -32805,7 +32806,7 @@
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="15"/>
@@ -32815,7 +32816,7 @@
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="15"/>
@@ -32843,7 +32844,7 @@
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="15"/>
@@ -32853,7 +32854,7 @@
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="15"/>
@@ -32867,7 +32868,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="24">
         <v>3</v>
@@ -32881,7 +32882,7 @@
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -32891,7 +32892,7 @@
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -32901,7 +32902,7 @@
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="15"/>
@@ -32915,7 +32916,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="24">
         <v>5</v>
@@ -32929,7 +32930,7 @@
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
@@ -32939,7 +32940,7 @@
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
@@ -32949,7 +32950,7 @@
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -32963,7 +32964,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="24">
         <v>3</v>
@@ -32977,7 +32978,7 @@
       <c r="A21" s="20"/>
       <c r="B21" s="15"/>
       <c r="C21" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -32987,7 +32988,7 @@
       <c r="A22" s="20"/>
       <c r="B22" s="15"/>
       <c r="C22" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
@@ -32997,7 +32998,7 @@
       <c r="A23" s="20"/>
       <c r="B23" s="15"/>
       <c r="C23" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -33007,7 +33008,7 @@
       <c r="A24" s="20"/>
       <c r="B24" s="15"/>
       <c r="C24" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
@@ -33021,7 +33022,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="24">
         <v>2</v>
@@ -33035,7 +33036,7 @@
       <c r="A26" s="20"/>
       <c r="B26" s="15"/>
       <c r="C26" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -33045,7 +33046,7 @@
       <c r="A27" s="20"/>
       <c r="B27" s="15"/>
       <c r="C27" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
@@ -33059,7 +33060,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" s="28">
         <v>8</v>
@@ -33073,7 +33074,7 @@
       <c r="A29" s="21"/>
       <c r="B29" s="15"/>
       <c r="C29" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
@@ -33083,7 +33084,7 @@
       <c r="A30" s="21"/>
       <c r="B30" s="15"/>
       <c r="C30" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
@@ -33093,7 +33094,7 @@
       <c r="A31" s="21"/>
       <c r="B31" s="15"/>
       <c r="C31" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -33103,7 +33104,7 @@
       <c r="A32" s="21"/>
       <c r="B32" s="15"/>
       <c r="C32" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -33117,7 +33118,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33" s="28">
         <v>8</v>
@@ -33131,7 +33132,7 @@
       <c r="A34" s="21"/>
       <c r="B34" s="15"/>
       <c r="C34" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -33141,7 +33142,7 @@
       <c r="A35" s="21"/>
       <c r="B35" s="15"/>
       <c r="C35" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -33155,7 +33156,7 @@
         <v>5</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="28">
         <v>13</v>
@@ -33170,7 +33171,7 @@
       <c r="A37" s="20"/>
       <c r="B37" s="15"/>
       <c r="C37" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
@@ -33180,7 +33181,7 @@
       <c r="A38" s="20"/>
       <c r="B38" s="12"/>
       <c r="C38" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
@@ -33190,7 +33191,7 @@
       <c r="A39" s="20"/>
       <c r="B39" s="12"/>
       <c r="C39" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
@@ -33200,7 +33201,7 @@
       <c r="A40" s="20"/>
       <c r="B40" s="12"/>
       <c r="C40" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
@@ -36175,23 +36176,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006D06A881EF84BF4D9C2E0A241D74C9AB" ma:contentTypeVersion="7" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="1106f65a84b95f72a5779278a76493c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cff42edc-c61c-4f4e-a404-7f98bf7ffabe" xmlns:ns4="cad3c75a-58d7-40e3-abd0-865ba3ea7957" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2bfd2deab1e7c17a6fd680c7b0ccc663" ns3:_="" ns4:_="">
     <xsd:import namespace="cff42edc-c61c-4f4e-a404-7f98bf7ffabe"/>
@@ -36374,10 +36358,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49D81426-816F-45B2-85EE-2F928428D617}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{267D6792-3005-46D7-935D-40B1E3BB51A9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cff42edc-c61c-4f4e-a404-7f98bf7ffabe"/>
+    <ds:schemaRef ds:uri="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -36400,20 +36412,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{267D6792-3005-46D7-935D-40B1E3BB51A9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49D81426-816F-45B2-85EE-2F928428D617}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cff42edc-c61c-4f4e-a404-7f98bf7ffabe"/>
-    <ds:schemaRef ds:uri="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>